<commit_message>
05.09.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Price list September 2020.xlsx
+++ b/2020/Others/Price list September 2020.xlsx
@@ -637,7 +637,7 @@
         <xdr:cNvPr id="2" name="Group 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -658,7 +658,7 @@
           <xdr:cNvPr id="3" name="Freeform 21">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -864,7 +864,7 @@
           <xdr:cNvPr id="4" name="Freeform 22">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1965,7 +1965,7 @@
           <xdr:cNvPr id="5" name="Freeform 23">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2405,7 +2405,7 @@
           <xdr:cNvPr id="6" name="Freeform 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2465,7 +2465,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2482,7 +2482,7 @@
           <xdr:cNvPr id="7" name="Freeform 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2545,7 +2545,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2562,7 +2562,7 @@
           <xdr:cNvPr id="8" name="Freeform 26">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2622,7 +2622,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2655,7 +2655,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2667,7 +2667,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2945,7 +2945,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2956,7 +2956,7 @@
   <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N13:N15"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
12.09.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Price list September 2020.xlsx
+++ b/2020/Others/Price list September 2020.xlsx
@@ -637,7 +637,7 @@
         <xdr:cNvPr id="2" name="Group 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -658,7 +658,7 @@
           <xdr:cNvPr id="3" name="Freeform 21">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -864,7 +864,7 @@
           <xdr:cNvPr id="4" name="Freeform 22">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1965,7 +1965,7 @@
           <xdr:cNvPr id="5" name="Freeform 23">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2405,7 +2405,7 @@
           <xdr:cNvPr id="6" name="Freeform 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2465,7 +2465,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2482,7 +2482,7 @@
           <xdr:cNvPr id="7" name="Freeform 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2545,7 +2545,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2562,7 +2562,7 @@
           <xdr:cNvPr id="8" name="Freeform 26">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2622,7 +2622,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2655,7 +2655,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2667,7 +2667,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2945,7 +2945,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2955,8 +2955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="L54" sqref="L54"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
23.09.2020 Before All Update
</commit_message>
<xml_diff>
--- a/2020/Others/Price list September 2020.xlsx
+++ b/2020/Others/Price list September 2020.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="82">
   <si>
     <t>Model</t>
   </si>
@@ -48,15 +48,9 @@
     <t>L25i</t>
   </si>
   <si>
-    <t>T130</t>
-  </si>
-  <si>
     <t>V44</t>
   </si>
   <si>
-    <t>V135</t>
-  </si>
-  <si>
     <t>V155</t>
   </si>
   <si>
@@ -177,9 +171,6 @@
     <t>i30_SKD</t>
   </si>
   <si>
-    <t>i60</t>
-  </si>
-  <si>
     <t>i65_SKD</t>
   </si>
   <si>
@@ -192,21 +183,12 @@
     <t>i74_SKD</t>
   </si>
   <si>
-    <t>i90</t>
-  </si>
-  <si>
-    <t>i90_2GB</t>
-  </si>
-  <si>
     <t>i95_SKD</t>
   </si>
   <si>
     <t>i97_SKD</t>
   </si>
   <si>
-    <t>L40_SKD</t>
-  </si>
-  <si>
     <t>L45</t>
   </si>
   <si>
@@ -249,12 +231,6 @@
     <t>V141_SKD</t>
   </si>
   <si>
-    <t>V145</t>
-  </si>
-  <si>
-    <t>V150</t>
-  </si>
-  <si>
     <t>Z12_SKD</t>
   </si>
   <si>
@@ -291,7 +267,10 @@
     <t>i99</t>
   </si>
   <si>
-    <t>September</t>
+    <t>i98</t>
+  </si>
+  <si>
+    <t>Z28_SKD</t>
   </si>
 </sst>
 </file>
@@ -377,12 +356,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="11">
@@ -513,7 +498,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -550,10 +535,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -592,11 +583,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -637,7 +631,7 @@
         <xdr:cNvPr id="2" name="Group 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -658,7 +652,7 @@
           <xdr:cNvPr id="3" name="Freeform 21">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -864,7 +858,7 @@
           <xdr:cNvPr id="4" name="Freeform 22">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1965,7 +1959,7 @@
           <xdr:cNvPr id="5" name="Freeform 23">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2405,7 +2399,7 @@
           <xdr:cNvPr id="6" name="Freeform 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2465,7 +2459,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2482,7 +2476,7 @@
           <xdr:cNvPr id="7" name="Freeform 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2545,7 +2539,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2562,7 +2556,7 @@
           <xdr:cNvPr id="8" name="Freeform 26">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2622,7 +2616,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2640,22 +2634,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>889997</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>933450</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>385793</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2667,7 +2661,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2677,8 +2671,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2552700" y="9525"/>
-          <a:ext cx="404222" cy="409575"/>
+          <a:off x="2638425" y="19050"/>
+          <a:ext cx="361950" cy="366743"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2945,7 +2939,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2955,8 +2949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L53" sqref="L53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2974,58 +2968,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25">
-      <c r="A1" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="A1" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
+      <c r="A2" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
     </row>
     <row r="4" spans="1:15" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A4" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
+      <c r="A4" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="H4" s="30">
-        <v>2020</v>
-      </c>
-      <c r="I4" s="31"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="34"/>
     </row>
     <row r="5" spans="1:15" ht="21" customHeight="1">
       <c r="A5" s="12" t="s">
@@ -3038,7 +3028,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="12" t="s">
@@ -3051,12 +3041,12 @@
         <v>2</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" s="5">
         <v>780</v>
@@ -3067,7 +3057,7 @@
       <c r="D6" s="5"/>
       <c r="E6" s="6"/>
       <c r="F6" s="8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G6" s="7">
         <v>6470</v>
@@ -3092,14 +3082,10 @@
       <c r="D7" s="5"/>
       <c r="E7" s="6"/>
       <c r="F7" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="G7" s="7">
-        <v>6570</v>
-      </c>
-      <c r="H7" s="7">
-        <v>6990</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:15" ht="20.100000000000001" customHeight="1">
@@ -3115,19 +3101,19 @@
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
       <c r="F8" s="8" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="G8" s="7">
-        <v>1070</v>
+        <v>6570</v>
       </c>
       <c r="H8" s="7">
-        <v>1160</v>
+        <v>6990</v>
       </c>
       <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B9" s="5">
         <v>740</v>
@@ -3138,19 +3124,19 @@
       <c r="D9" s="5"/>
       <c r="E9" s="6"/>
       <c r="F9" s="8" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G9" s="7">
+        <v>1070</v>
+      </c>
+      <c r="H9" s="7">
         <v>1160</v>
-      </c>
-      <c r="H9" s="7">
-        <v>1250</v>
       </c>
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" s="5">
         <v>740</v>
@@ -3161,19 +3147,19 @@
       <c r="D10" s="5"/>
       <c r="E10" s="6"/>
       <c r="F10" s="8" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="G10" s="7">
-        <v>1010</v>
+        <v>1160</v>
       </c>
       <c r="H10" s="7">
-        <v>1090</v>
+        <v>1250</v>
       </c>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" s="5">
         <v>790</v>
@@ -3184,19 +3170,19 @@
       <c r="D11" s="5"/>
       <c r="E11" s="6"/>
       <c r="F11" s="9" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="G11" s="7">
-        <v>1040</v>
+        <v>1010</v>
       </c>
       <c r="H11" s="7">
-        <v>1130</v>
+        <v>1090</v>
       </c>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" s="5">
         <v>800</v>
@@ -3209,7 +3195,7 @@
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G12" s="7">
         <v>970</v>
@@ -3221,7 +3207,7 @@
     </row>
     <row r="13" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B13" s="5">
         <v>760</v>
@@ -3232,7 +3218,7 @@
       <c r="D13" s="5"/>
       <c r="E13" s="6"/>
       <c r="F13" s="8" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G13" s="7">
         <v>960</v>
@@ -3244,7 +3230,7 @@
     </row>
     <row r="14" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B14" s="7">
         <v>970</v>
@@ -3255,7 +3241,7 @@
       <c r="D14" s="5"/>
       <c r="E14" s="6"/>
       <c r="F14" s="8" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="G14" s="7">
         <v>1080</v>
@@ -3267,7 +3253,7 @@
     </row>
     <row r="15" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" s="5">
         <v>920</v>
@@ -3278,7 +3264,7 @@
       <c r="D15" s="5"/>
       <c r="E15" s="6"/>
       <c r="F15" s="8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G15" s="7">
         <v>5750</v>
@@ -3290,12 +3276,12 @@
         <v>700</v>
       </c>
       <c r="O15" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16" s="5">
         <v>915</v>
@@ -3306,7 +3292,7 @@
       <c r="D16" s="5"/>
       <c r="E16" s="6"/>
       <c r="F16" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G16" s="7">
         <v>1190</v>
@@ -3320,7 +3306,7 @@
     </row>
     <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B17" s="5">
         <v>920</v>
@@ -3331,7 +3317,7 @@
       <c r="D17" s="5"/>
       <c r="E17" s="6"/>
       <c r="F17" s="8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="G17" s="7">
         <v>1100</v>
@@ -3356,19 +3342,19 @@
       <c r="D18" s="5"/>
       <c r="E18" s="6"/>
       <c r="F18" s="8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G18" s="7">
-        <v>1250</v>
+        <v>1370</v>
       </c>
       <c r="H18" s="7">
-        <v>1350</v>
+        <v>1490</v>
       </c>
       <c r="I18" s="5"/>
     </row>
     <row r="19" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B19" s="5">
         <v>845</v>
@@ -3380,20 +3366,20 @@
         <v>25</v>
       </c>
       <c r="E19" s="6"/>
-      <c r="F19" s="8" t="s">
-        <v>11</v>
+      <c r="F19" s="16" t="s">
+        <v>37</v>
       </c>
       <c r="G19" s="7">
-        <v>1370</v>
+        <v>1220</v>
       </c>
       <c r="H19" s="7">
-        <v>1490</v>
+        <v>1320</v>
       </c>
       <c r="I19" s="5"/>
     </row>
     <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B20" s="5">
         <v>820</v>
@@ -3404,19 +3390,19 @@
       <c r="D20" s="5"/>
       <c r="E20" s="6"/>
       <c r="F20" s="8" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="G20" s="7">
-        <v>1220</v>
+        <v>3610</v>
       </c>
       <c r="H20" s="7">
-        <v>1320</v>
+        <v>3890</v>
       </c>
       <c r="I20" s="5"/>
     </row>
     <row r="21" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" s="5">
         <v>880</v>
@@ -3426,20 +3412,20 @@
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="6"/>
-      <c r="F21" s="17" t="s">
-        <v>70</v>
+      <c r="F21" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="G21" s="7">
-        <v>3610</v>
+        <v>3890</v>
       </c>
       <c r="H21" s="7">
-        <v>3890</v>
+        <v>4190</v>
       </c>
       <c r="I21" s="5"/>
     </row>
     <row r="22" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B22" s="7">
         <v>900</v>
@@ -3450,19 +3436,19 @@
       <c r="D22" s="5"/>
       <c r="E22" s="6"/>
       <c r="F22" s="8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G22" s="7">
-        <v>3890</v>
+        <v>4280</v>
       </c>
       <c r="H22" s="7">
-        <v>4190</v>
+        <v>4590</v>
       </c>
       <c r="I22" s="5"/>
     </row>
     <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A23" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B23" s="7">
         <v>1040</v>
@@ -3473,19 +3459,19 @@
       <c r="D23" s="5"/>
       <c r="E23" s="6"/>
       <c r="F23" s="8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G23" s="7">
-        <v>4280</v>
+        <v>4180</v>
       </c>
       <c r="H23" s="7">
-        <v>4590</v>
+        <v>4490</v>
       </c>
       <c r="I23" s="5"/>
     </row>
     <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B24" s="7">
         <v>930</v>
@@ -3496,19 +3482,19 @@
       <c r="D24" s="5"/>
       <c r="E24" s="6"/>
       <c r="F24" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G24" s="7">
-        <v>5020</v>
+        <v>5390</v>
       </c>
       <c r="H24" s="7">
-        <v>5390</v>
+        <v>5790</v>
       </c>
       <c r="I24" s="5"/>
     </row>
     <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B25" s="7">
         <v>940</v>
@@ -3519,19 +3505,19 @@
       <c r="D25" s="5"/>
       <c r="E25" s="6"/>
       <c r="F25" s="8" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="G25" s="7">
-        <v>4180</v>
+        <v>3560</v>
       </c>
       <c r="H25" s="7">
-        <v>4490</v>
+        <v>3840</v>
       </c>
       <c r="I25" s="5"/>
     </row>
     <row r="26" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B26" s="5">
         <v>1170</v>
@@ -3542,19 +3528,19 @@
       <c r="D26" s="5"/>
       <c r="E26" s="6"/>
       <c r="F26" s="8" t="s">
-        <v>74</v>
+        <v>13</v>
       </c>
       <c r="G26" s="7">
-        <v>5560</v>
+        <v>3340</v>
       </c>
       <c r="H26" s="7">
-        <v>5990</v>
+        <v>3590</v>
       </c>
       <c r="I26" s="5"/>
     </row>
     <row r="27" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B27" s="7">
         <v>870</v>
@@ -3565,19 +3551,19 @@
       <c r="D27" s="5"/>
       <c r="E27" s="6"/>
       <c r="F27" s="8" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="G27" s="7">
-        <v>6090</v>
+        <v>4500</v>
       </c>
       <c r="H27" s="7">
-        <v>6590</v>
+        <v>4790</v>
       </c>
       <c r="I27" s="5"/>
     </row>
     <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B28" s="7">
         <v>1020</v>
@@ -3588,19 +3574,19 @@
       <c r="D28" s="5"/>
       <c r="E28" s="6"/>
       <c r="F28" s="8" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="G28" s="7">
-        <v>5390</v>
+        <v>3620</v>
       </c>
       <c r="H28" s="7">
-        <v>5790</v>
+        <v>3890</v>
       </c>
       <c r="I28" s="5"/>
     </row>
     <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B29" s="7">
         <v>2780</v>
@@ -3613,19 +3599,19 @@
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="8" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="G29" s="7">
-        <v>3560</v>
+        <v>4080</v>
       </c>
       <c r="H29" s="7">
-        <v>3840</v>
+        <v>4390</v>
       </c>
       <c r="I29" s="5"/>
     </row>
     <row r="30" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B30" s="7">
         <v>2770</v>
@@ -3638,19 +3624,19 @@
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="8" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="G30" s="7">
-        <v>3340</v>
+        <v>4220</v>
       </c>
       <c r="H30" s="7">
-        <v>3590</v>
+        <v>4540</v>
       </c>
       <c r="I30" s="5"/>
     </row>
     <row r="31" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A31" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B31" s="7">
         <v>4050</v>
@@ -3661,19 +3647,19 @@
       <c r="D31" s="5"/>
       <c r="E31" s="6"/>
       <c r="F31" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G31" s="7">
-        <v>4500</v>
+        <v>3640</v>
       </c>
       <c r="H31" s="7">
-        <v>4790</v>
+        <v>3890</v>
       </c>
       <c r="I31" s="5"/>
     </row>
     <row r="32" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A32" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B32" s="7">
         <v>6540</v>
@@ -3684,19 +3670,19 @@
       <c r="D32" s="5"/>
       <c r="E32" s="6"/>
       <c r="F32" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G32" s="7">
-        <v>3620</v>
+        <v>3710</v>
       </c>
       <c r="H32" s="7">
-        <v>3890</v>
+        <v>3990</v>
       </c>
       <c r="I32" s="5"/>
     </row>
     <row r="33" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="8" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B33" s="7">
         <v>4150</v>
@@ -3707,19 +3693,21 @@
       <c r="D33" s="5"/>
       <c r="E33" s="6"/>
       <c r="F33" s="8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G33" s="7">
-        <v>4080</v>
+        <v>7350</v>
       </c>
       <c r="H33" s="7">
-        <v>4390</v>
-      </c>
-      <c r="I33" s="5"/>
+        <v>7990</v>
+      </c>
+      <c r="I33" s="5">
+        <v>700</v>
+      </c>
     </row>
     <row r="34" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B34" s="7">
         <v>5290</v>
@@ -3730,19 +3718,21 @@
       <c r="D34" s="5"/>
       <c r="E34" s="6"/>
       <c r="F34" s="8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G34" s="7">
-        <v>4220</v>
+        <v>7890</v>
       </c>
       <c r="H34" s="7">
-        <v>4540</v>
-      </c>
-      <c r="I34" s="5"/>
+        <v>8490</v>
+      </c>
+      <c r="I34" s="5">
+        <v>300</v>
+      </c>
     </row>
     <row r="35" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B35" s="7">
         <v>5010</v>
@@ -3753,19 +3743,19 @@
       <c r="D35" s="5"/>
       <c r="E35" s="6"/>
       <c r="F35" s="8" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="G35" s="7">
-        <v>3640</v>
+        <v>7790</v>
       </c>
       <c r="H35" s="7">
-        <v>3890</v>
+        <v>8290</v>
       </c>
       <c r="I35" s="5"/>
     </row>
     <row r="36" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A36" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B36" s="7">
         <v>5170</v>
@@ -3776,193 +3766,153 @@
       <c r="D36" s="5"/>
       <c r="E36" s="6"/>
       <c r="F36" s="8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G36" s="7">
-        <v>3710</v>
+        <v>8310</v>
       </c>
       <c r="H36" s="7">
-        <v>3990</v>
+        <v>8990</v>
       </c>
       <c r="I36" s="5"/>
     </row>
     <row r="37" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A37" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B37" s="7">
-        <v>7075</v>
+        <v>5750</v>
       </c>
       <c r="C37" s="7">
-        <v>7575</v>
-      </c>
-      <c r="D37" s="5"/>
+        <v>6190</v>
+      </c>
+      <c r="D37" s="5">
+        <v>550</v>
+      </c>
       <c r="E37" s="6"/>
       <c r="F37" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G37" s="7">
-        <v>7350</v>
+        <v>8310</v>
       </c>
       <c r="H37" s="7">
-        <v>7990</v>
-      </c>
-      <c r="I37" s="5">
-        <v>700</v>
-      </c>
+        <v>8990</v>
+      </c>
+      <c r="I37" s="5"/>
     </row>
     <row r="38" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A38" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B38" s="7">
-        <v>5750</v>
-      </c>
-      <c r="C38" s="7">
-        <v>6190</v>
-      </c>
-      <c r="D38" s="5">
-        <v>550</v>
-      </c>
+      <c r="A38" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="18">
+        <v>4990</v>
+      </c>
+      <c r="C38" s="18">
+        <v>5290</v>
+      </c>
+      <c r="D38" s="19"/>
       <c r="E38" s="6"/>
       <c r="F38" s="8" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="G38" s="7">
-        <v>7890</v>
+        <v>8450</v>
       </c>
       <c r="H38" s="7">
-        <v>8490</v>
-      </c>
-      <c r="I38" s="5">
-        <v>300</v>
-      </c>
+        <v>8990</v>
+      </c>
+      <c r="I38" s="5"/>
     </row>
     <row r="39" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B39" s="7">
-        <v>4990</v>
+        <v>5550</v>
       </c>
       <c r="C39" s="7">
-        <v>5290</v>
+        <v>5990</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="6"/>
       <c r="F39" s="8" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="G39" s="7">
-        <v>7790</v>
+        <v>9300</v>
       </c>
       <c r="H39" s="7">
-        <v>8290</v>
+        <v>9790</v>
       </c>
       <c r="I39" s="5"/>
     </row>
     <row r="40" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B40" s="7">
-        <v>5550</v>
+        <v>5940</v>
       </c>
       <c r="C40" s="7">
-        <v>5990</v>
+        <v>6390</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="6"/>
       <c r="F40" s="8" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G40" s="7">
-        <v>8310</v>
+        <v>10340</v>
       </c>
       <c r="H40" s="7">
-        <v>8990</v>
+        <v>10990</v>
       </c>
       <c r="I40" s="5"/>
     </row>
     <row r="41" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B41" s="7">
-        <v>5940</v>
+        <v>5510</v>
       </c>
       <c r="C41" s="7">
-        <v>6390</v>
+        <v>5890</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="6"/>
-      <c r="F41" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="G41" s="7">
-        <v>8310</v>
-      </c>
-      <c r="H41" s="7">
-        <v>8990</v>
-      </c>
+      <c r="F41" s="8"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
       <c r="I41" s="5"/>
     </row>
     <row r="42" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A42" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B42" s="7">
-        <v>7890</v>
-      </c>
-      <c r="C42" s="7">
-        <v>8490</v>
-      </c>
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
       <c r="D42" s="5"/>
       <c r="E42" s="6"/>
-      <c r="F42" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="G42" s="7">
-        <v>9300</v>
-      </c>
-      <c r="H42" s="7">
-        <v>9790</v>
-      </c>
+      <c r="F42" s="8"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
       <c r="I42" s="5"/>
     </row>
     <row r="43" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A43" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B43" s="7">
-        <v>9100</v>
-      </c>
-      <c r="C43" s="7">
-        <v>9790</v>
-      </c>
+      <c r="A43" s="8"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
       <c r="D43" s="5"/>
       <c r="E43" s="6"/>
-      <c r="F43" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="G43" s="7">
-        <v>10340</v>
-      </c>
-      <c r="H43" s="7">
-        <v>10990</v>
-      </c>
+      <c r="F43" s="8"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
       <c r="I43" s="5"/>
     </row>
     <row r="44" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A44" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B44" s="7">
-        <v>5510</v>
-      </c>
-      <c r="C44" s="7">
-        <v>5890</v>
-      </c>
+      <c r="A44" s="8"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
       <c r="D44" s="5"/>
       <c r="E44" s="6"/>
       <c r="F44" s="8"/>
@@ -3971,33 +3921,33 @@
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B45" s="19"/>
-      <c r="C45" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="I45" s="23"/>
+      <c r="A45" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="21"/>
+      <c r="C45" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I45" s="25"/>
       <c r="J45" s="2"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="20"/>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="24"/>
-      <c r="I46" s="25"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="27"/>
       <c r="J46" s="2"/>
     </row>
     <row r="47" spans="1:10">
@@ -4015,7 +3965,7 @@
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A4:D4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="F4:I4"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
27.09.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Price list September 2020.xlsx
+++ b/2020/Others/Price list September 2020.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
   <si>
     <t>Model</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Distributor: Symphony (Mobile Handset) Edison-Group</t>
   </si>
   <si>
-    <t>+8801312-116768</t>
-  </si>
-  <si>
     <t xml:space="preserve">    mugdhocorporation@gmail.com</t>
   </si>
   <si>
@@ -271,6 +268,15 @@
   </si>
   <si>
     <t>Z28_SKD</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+8801312-116768 </t>
+  </si>
+  <si>
+    <t>DSR Name</t>
   </si>
 </sst>
 </file>
@@ -370,7 +376,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -456,19 +462,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -547,30 +540,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -583,13 +552,37 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -616,13 +609,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>209297</xdr:colOff>
+      <xdr:colOff>165212</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>42755</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>968613</xdr:colOff>
+      <xdr:colOff>968610</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>114587</xdr:rowOff>
     </xdr:to>
@@ -631,7 +624,7 @@
         <xdr:cNvPr id="2" name="Group 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -641,10 +634,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="209297" y="10977455"/>
-          <a:ext cx="5921866" cy="271857"/>
-          <a:chOff x="248" y="249"/>
-          <a:chExt cx="403" cy="292"/>
+          <a:off x="165212" y="10977455"/>
+          <a:ext cx="5965948" cy="271857"/>
+          <a:chOff x="245" y="249"/>
+          <a:chExt cx="406" cy="292"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
@@ -652,7 +645,7 @@
           <xdr:cNvPr id="3" name="Freeform 21">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -858,7 +851,7 @@
           <xdr:cNvPr id="4" name="Freeform 22">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1959,7 +1952,7 @@
           <xdr:cNvPr id="5" name="Freeform 23">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1969,7 +1962,7 @@
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="248" y="305"/>
+            <a:off x="245" y="305"/>
             <a:ext cx="16" cy="205"/>
           </a:xfrm>
           <a:custGeom>
@@ -2393,13 +2386,20 @@
             </a:solidFill>
           </a:ln>
         </xdr:spPr>
+        <xdr:txBody>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </xdr:txBody>
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
           <xdr:cNvPr id="6" name="Freeform 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2459,7 +2459,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2476,7 +2476,7 @@
           <xdr:cNvPr id="7" name="Freeform 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2539,7 +2539,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2556,7 +2556,7 @@
           <xdr:cNvPr id="8" name="Freeform 26">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2616,7 +2616,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2649,7 +2649,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2661,7 +2661,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2939,7 +2939,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2949,8 +2949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L53" sqref="L53"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2968,54 +2968,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25">
-      <c r="A1" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
+      <c r="A1" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
     </row>
     <row r="4" spans="1:15" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="34"/>
+      <c r="F4" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="25"/>
     </row>
     <row r="5" spans="1:15" ht="21" customHeight="1">
       <c r="A5" s="12" t="s">
@@ -3028,7 +3030,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="12" t="s">
@@ -3041,7 +3043,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="20.100000000000001" customHeight="1">
@@ -3057,7 +3059,7 @@
       <c r="D6" s="5"/>
       <c r="E6" s="6"/>
       <c r="F6" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" s="7">
         <v>6470</v>
@@ -3082,10 +3084,14 @@
       <c r="D7" s="5"/>
       <c r="E7" s="6"/>
       <c r="F7" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+        <v>79</v>
+      </c>
+      <c r="G7" s="7">
+        <v>5855</v>
+      </c>
+      <c r="H7" s="7">
+        <v>6295</v>
+      </c>
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:15" ht="20.100000000000001" customHeight="1">
@@ -3101,7 +3107,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
       <c r="F8" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G8" s="7">
         <v>6570</v>
@@ -3113,7 +3119,7 @@
     </row>
     <row r="9" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="5">
         <v>740</v>
@@ -3136,7 +3142,7 @@
     </row>
     <row r="10" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="5">
         <v>740</v>
@@ -3147,7 +3153,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="6"/>
       <c r="F10" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G10" s="7">
         <v>1160</v>
@@ -3182,7 +3188,7 @@
     </row>
     <row r="12" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="5">
         <v>800</v>
@@ -3195,7 +3201,7 @@
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G12" s="7">
         <v>970</v>
@@ -3207,7 +3213,7 @@
     </row>
     <row r="13" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="5">
         <v>760</v>
@@ -3218,7 +3224,7 @@
       <c r="D13" s="5"/>
       <c r="E13" s="6"/>
       <c r="F13" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G13" s="7">
         <v>960</v>
@@ -3230,7 +3236,7 @@
     </row>
     <row r="14" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="7">
         <v>970</v>
@@ -3241,7 +3247,7 @@
       <c r="D14" s="5"/>
       <c r="E14" s="6"/>
       <c r="F14" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G14" s="7">
         <v>1080</v>
@@ -3253,7 +3259,7 @@
     </row>
     <row r="15" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="5">
         <v>920</v>
@@ -3264,7 +3270,7 @@
       <c r="D15" s="5"/>
       <c r="E15" s="6"/>
       <c r="F15" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G15" s="7">
         <v>5750</v>
@@ -3276,7 +3282,7 @@
         <v>700</v>
       </c>
       <c r="O15" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="20.100000000000001" customHeight="1">
@@ -3292,7 +3298,7 @@
       <c r="D16" s="5"/>
       <c r="E16" s="6"/>
       <c r="F16" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G16" s="7">
         <v>1190</v>
@@ -3317,7 +3323,7 @@
       <c r="D17" s="5"/>
       <c r="E17" s="6"/>
       <c r="F17" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G17" s="7">
         <v>1100</v>
@@ -3367,7 +3373,7 @@
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G19" s="7">
         <v>1220</v>
@@ -3379,7 +3385,7 @@
     </row>
     <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" s="5">
         <v>820</v>
@@ -3390,7 +3396,7 @@
       <c r="D20" s="5"/>
       <c r="E20" s="6"/>
       <c r="F20" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G20" s="7">
         <v>3610</v>
@@ -3413,7 +3419,7 @@
       <c r="D21" s="5"/>
       <c r="E21" s="6"/>
       <c r="F21" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G21" s="7">
         <v>3890</v>
@@ -3436,7 +3442,7 @@
       <c r="D22" s="5"/>
       <c r="E22" s="6"/>
       <c r="F22" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G22" s="7">
         <v>4280</v>
@@ -3448,7 +3454,7 @@
     </row>
     <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A23" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" s="7">
         <v>1040</v>
@@ -3459,7 +3465,7 @@
       <c r="D23" s="5"/>
       <c r="E23" s="6"/>
       <c r="F23" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G23" s="7">
         <v>4180</v>
@@ -3494,7 +3500,7 @@
     </row>
     <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" s="7">
         <v>940</v>
@@ -3517,7 +3523,7 @@
     </row>
     <row r="26" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="5">
         <v>1170</v>
@@ -3540,7 +3546,7 @@
     </row>
     <row r="27" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" s="7">
         <v>870</v>
@@ -3551,7 +3557,7 @@
       <c r="D27" s="5"/>
       <c r="E27" s="6"/>
       <c r="F27" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G27" s="7">
         <v>4500</v>
@@ -3563,7 +3569,7 @@
     </row>
     <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" s="7">
         <v>1020</v>
@@ -3574,7 +3580,7 @@
       <c r="D28" s="5"/>
       <c r="E28" s="6"/>
       <c r="F28" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G28" s="7">
         <v>3620</v>
@@ -3586,7 +3592,7 @@
     </row>
     <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" s="7">
         <v>2780</v>
@@ -3599,7 +3605,7 @@
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G29" s="7">
         <v>4080</v>
@@ -3611,7 +3617,7 @@
     </row>
     <row r="30" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B30" s="7">
         <v>2770</v>
@@ -3624,7 +3630,7 @@
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G30" s="7">
         <v>4220</v>
@@ -3636,7 +3642,7 @@
     </row>
     <row r="31" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A31" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B31" s="7">
         <v>4050</v>
@@ -3647,7 +3653,7 @@
       <c r="D31" s="5"/>
       <c r="E31" s="6"/>
       <c r="F31" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G31" s="7">
         <v>3640</v>
@@ -3659,7 +3665,7 @@
     </row>
     <row r="32" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A32" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B32" s="7">
         <v>6540</v>
@@ -3670,7 +3676,7 @@
       <c r="D32" s="5"/>
       <c r="E32" s="6"/>
       <c r="F32" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G32" s="7">
         <v>3710</v>
@@ -3682,7 +3688,7 @@
     </row>
     <row r="33" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B33" s="7">
         <v>4150</v>
@@ -3693,7 +3699,7 @@
       <c r="D33" s="5"/>
       <c r="E33" s="6"/>
       <c r="F33" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G33" s="7">
         <v>7350</v>
@@ -3707,7 +3713,7 @@
     </row>
     <row r="34" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B34" s="7">
         <v>5290</v>
@@ -3718,7 +3724,7 @@
       <c r="D34" s="5"/>
       <c r="E34" s="6"/>
       <c r="F34" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G34" s="7">
         <v>7890</v>
@@ -3732,7 +3738,7 @@
     </row>
     <row r="35" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B35" s="7">
         <v>5010</v>
@@ -3743,7 +3749,7 @@
       <c r="D35" s="5"/>
       <c r="E35" s="6"/>
       <c r="F35" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G35" s="7">
         <v>7790</v>
@@ -3755,7 +3761,7 @@
     </row>
     <row r="36" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A36" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B36" s="7">
         <v>5170</v>
@@ -3766,7 +3772,7 @@
       <c r="D36" s="5"/>
       <c r="E36" s="6"/>
       <c r="F36" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G36" s="7">
         <v>8310</v>
@@ -3778,7 +3784,7 @@
     </row>
     <row r="37" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A37" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B37" s="7">
         <v>5750</v>
@@ -3791,7 +3797,7 @@
       </c>
       <c r="E37" s="6"/>
       <c r="F37" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G37" s="7">
         <v>8310</v>
@@ -3803,7 +3809,7 @@
     </row>
     <row r="38" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B38" s="18">
         <v>4990</v>
@@ -3811,10 +3817,12 @@
       <c r="C38" s="18">
         <v>5290</v>
       </c>
-      <c r="D38" s="19"/>
+      <c r="D38" s="19" t="s">
+        <v>81</v>
+      </c>
       <c r="E38" s="6"/>
       <c r="F38" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G38" s="7">
         <v>8450</v>
@@ -3826,7 +3834,7 @@
     </row>
     <row r="39" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B39" s="7">
         <v>5550</v>
@@ -3837,7 +3845,7 @@
       <c r="D39" s="5"/>
       <c r="E39" s="6"/>
       <c r="F39" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G39" s="7">
         <v>9300</v>
@@ -3849,7 +3857,7 @@
     </row>
     <row r="40" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B40" s="7">
         <v>5940</v>
@@ -3860,7 +3868,7 @@
       <c r="D40" s="5"/>
       <c r="E40" s="6"/>
       <c r="F40" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G40" s="7">
         <v>10340</v>
@@ -3872,7 +3880,7 @@
     </row>
     <row r="41" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B41" s="7">
         <v>5510</v>
@@ -3921,33 +3929,33 @@
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="20" t="s">
+      <c r="A45" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" s="27"/>
+      <c r="C45" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="27"/>
+      <c r="H45" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B45" s="21"/>
-      <c r="C45" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
-      <c r="G45" s="21"/>
-      <c r="H45" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="I45" s="25"/>
+      <c r="I45" s="29"/>
       <c r="J45" s="2"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="22"/>
-      <c r="B46" s="23"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="23"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="23"/>
-      <c r="G46" s="23"/>
-      <c r="H46" s="26"/>
-      <c r="I46" s="27"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="31"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="31"/>
+      <c r="G46" s="31"/>
+      <c r="H46" s="32"/>
+      <c r="I46" s="33"/>
       <c r="J46" s="2"/>
     </row>
     <row r="47" spans="1:10">
@@ -3965,7 +3973,7 @@
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A4:D4"/>
-    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="G4:I4"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
27.09.2020 M C Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Price list September 2020.xlsx
+++ b/2020/Others/Price list September 2020.xlsx
@@ -540,6 +540,33 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -556,33 +583,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -624,7 +624,7 @@
         <xdr:cNvPr id="2" name="Group 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -645,7 +645,7 @@
           <xdr:cNvPr id="3" name="Freeform 21">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -851,7 +851,7 @@
           <xdr:cNvPr id="4" name="Freeform 22">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1952,7 +1952,7 @@
           <xdr:cNvPr id="5" name="Freeform 23">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2399,7 +2399,7 @@
           <xdr:cNvPr id="6" name="Freeform 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2459,7 +2459,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2476,7 +2476,7 @@
           <xdr:cNvPr id="7" name="Freeform 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2539,7 +2539,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2556,7 +2556,7 @@
           <xdr:cNvPr id="8" name="Freeform 26">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2616,7 +2616,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2649,7 +2649,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2661,7 +2661,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2939,7 +2939,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2949,8 +2949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2968,56 +2968,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
     </row>
     <row r="4" spans="1:15" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="25"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="34"/>
     </row>
     <row r="5" spans="1:15" ht="21" customHeight="1">
       <c r="A5" s="12" t="s">
@@ -3929,33 +3929,33 @@
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="26" t="s">
+      <c r="A45" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="B45" s="27"/>
-      <c r="C45" s="27" t="s">
+      <c r="B45" s="22"/>
+      <c r="C45" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="D45" s="27"/>
-      <c r="E45" s="27"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="27"/>
-      <c r="H45" s="28" t="s">
+      <c r="D45" s="22"/>
+      <c r="E45" s="22"/>
+      <c r="F45" s="22"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="I45" s="29"/>
+      <c r="I45" s="26"/>
       <c r="J45" s="2"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="30"/>
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="31"/>
-      <c r="H46" s="32"/>
-      <c r="I46" s="33"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="24"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="28"/>
       <c r="J46" s="2"/>
     </row>
     <row r="47" spans="1:10">

</xml_diff>

<commit_message>
30.09.2020 MC Capital Details
</commit_message>
<xml_diff>
--- a/2020/Others/Price list September 2020.xlsx
+++ b/2020/Others/Price list September 2020.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="85">
   <si>
     <t>Model</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>DSR Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -624,7 +627,7 @@
         <xdr:cNvPr id="2" name="Group 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -645,7 +648,7 @@
           <xdr:cNvPr id="3" name="Freeform 21">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -851,7 +854,7 @@
           <xdr:cNvPr id="4" name="Freeform 22">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1952,7 +1955,7 @@
           <xdr:cNvPr id="5" name="Freeform 23">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2399,7 +2402,7 @@
           <xdr:cNvPr id="6" name="Freeform 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2459,7 +2462,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2476,7 +2479,7 @@
           <xdr:cNvPr id="7" name="Freeform 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2539,7 +2542,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2556,7 +2559,7 @@
           <xdr:cNvPr id="8" name="Freeform 26">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2616,7 +2619,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2649,7 +2652,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2661,7 +2664,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2939,7 +2942,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2949,8 +2952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="O16" sqref="O13:P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3256,6 +3259,9 @@
         <v>1150</v>
       </c>
       <c r="I14" s="5"/>
+      <c r="K14" s="10" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="15" spans="1:15" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="8" t="s">

</xml_diff>

<commit_message>
03.10.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Price list September 2020.xlsx
+++ b/2020/Others/Price list September 2020.xlsx
@@ -627,7 +627,7 @@
         <xdr:cNvPr id="2" name="Group 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -648,7 +648,7 @@
           <xdr:cNvPr id="3" name="Freeform 21">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -854,7 +854,7 @@
           <xdr:cNvPr id="4" name="Freeform 22">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1955,7 +1955,7 @@
           <xdr:cNvPr id="5" name="Freeform 23">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2402,7 +2402,7 @@
           <xdr:cNvPr id="6" name="Freeform 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2462,7 +2462,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2479,7 +2479,7 @@
           <xdr:cNvPr id="7" name="Freeform 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2542,7 +2542,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2559,7 +2559,7 @@
           <xdr:cNvPr id="8" name="Freeform 26">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2619,7 +2619,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2652,7 +2652,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2664,7 +2664,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2942,7 +2942,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2952,8 +2952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="O16" sqref="O13:P16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
11.10.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Price list September 2020.xlsx
+++ b/2020/Others/Price list September 2020.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="86">
   <si>
     <t>Model</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>D74</t>
   </si>
 </sst>
 </file>
@@ -627,7 +630,7 @@
         <xdr:cNvPr id="2" name="Group 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -648,7 +651,7 @@
           <xdr:cNvPr id="3" name="Freeform 21">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -854,7 +857,7 @@
           <xdr:cNvPr id="4" name="Freeform 22">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1955,7 +1958,7 @@
           <xdr:cNvPr id="5" name="Freeform 23">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2402,7 +2405,7 @@
           <xdr:cNvPr id="6" name="Freeform 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2462,7 +2465,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2479,7 +2482,7 @@
           <xdr:cNvPr id="7" name="Freeform 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2542,7 +2545,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2559,7 +2562,7 @@
           <xdr:cNvPr id="8" name="Freeform 26">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2619,7 +2622,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2652,7 +2655,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2664,7 +2667,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2942,7 +2945,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2953,7 +2956,7 @@
   <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3575,13 +3578,13 @@
     </row>
     <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="8" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="B28" s="7">
-        <v>1020</v>
+        <v>890</v>
       </c>
       <c r="C28" s="7">
-        <v>1099</v>
+        <v>960</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="6"/>
@@ -3598,17 +3601,15 @@
     </row>
     <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="8" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B29" s="7">
-        <v>2780</v>
+        <v>1020</v>
       </c>
       <c r="C29" s="7">
-        <v>2990</v>
-      </c>
-      <c r="D29" s="5">
-        <v>450</v>
-      </c>
+        <v>1099</v>
+      </c>
+      <c r="D29" s="5"/>
       <c r="E29" s="6"/>
       <c r="F29" s="8" t="s">
         <v>59</v>
@@ -3623,10 +3624,10 @@
     </row>
     <row r="30" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" s="7">
-        <v>2770</v>
+        <v>2780</v>
       </c>
       <c r="C30" s="7">
         <v>2990</v>
@@ -3648,15 +3649,17 @@
     </row>
     <row r="31" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A31" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B31" s="7">
-        <v>4050</v>
+        <v>2770</v>
       </c>
       <c r="C31" s="7">
-        <v>4290</v>
-      </c>
-      <c r="D31" s="5"/>
+        <v>2990</v>
+      </c>
+      <c r="D31" s="5">
+        <v>450</v>
+      </c>
       <c r="E31" s="6"/>
       <c r="F31" s="8" t="s">
         <v>62</v>
@@ -3671,13 +3674,13 @@
     </row>
     <row r="32" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A32" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B32" s="7">
-        <v>6540</v>
+        <v>4050</v>
       </c>
       <c r="C32" s="7">
-        <v>6990</v>
+        <v>4290</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="6"/>
@@ -3694,13 +3697,13 @@
     </row>
     <row r="33" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="8" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="B33" s="7">
-        <v>4150</v>
+        <v>6540</v>
       </c>
       <c r="C33" s="7">
-        <v>4390</v>
+        <v>6990</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="6"/>
@@ -3719,13 +3722,13 @@
     </row>
     <row r="34" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="B34" s="7">
-        <v>5290</v>
+        <v>4150</v>
       </c>
       <c r="C34" s="7">
-        <v>5690</v>
+        <v>4390</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="6"/>
@@ -3744,13 +3747,13 @@
     </row>
     <row r="35" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B35" s="7">
-        <v>5010</v>
+        <v>5290</v>
       </c>
       <c r="C35" s="7">
-        <v>5390</v>
+        <v>5690</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="6"/>
@@ -3767,13 +3770,13 @@
     </row>
     <row r="36" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A36" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B36" s="7">
-        <v>5170</v>
+        <v>5010</v>
       </c>
       <c r="C36" s="7">
-        <v>5499</v>
+        <v>5390</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="6"/>
@@ -3790,17 +3793,15 @@
     </row>
     <row r="37" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A37" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B37" s="7">
-        <v>5750</v>
+        <v>5170</v>
       </c>
       <c r="C37" s="7">
-        <v>6190</v>
-      </c>
-      <c r="D37" s="5">
-        <v>550</v>
-      </c>
+        <v>5499</v>
+      </c>
+      <c r="D37" s="5"/>
       <c r="E37" s="6"/>
       <c r="F37" s="8" t="s">
         <v>71</v>
@@ -3815,16 +3816,16 @@
     </row>
     <row r="38" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38" s="18">
-        <v>4990</v>
+        <v>5750</v>
       </c>
       <c r="C38" s="18">
-        <v>5290</v>
-      </c>
-      <c r="D38" s="19" t="s">
-        <v>81</v>
+        <v>6190</v>
+      </c>
+      <c r="D38" s="19">
+        <v>550</v>
       </c>
       <c r="E38" s="6"/>
       <c r="F38" s="8" t="s">
@@ -3840,15 +3841,17 @@
     </row>
     <row r="39" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39" s="7">
-        <v>5550</v>
+        <v>4990</v>
       </c>
       <c r="C39" s="7">
-        <v>5990</v>
-      </c>
-      <c r="D39" s="5"/>
+        <v>5290</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>81</v>
+      </c>
       <c r="E39" s="6"/>
       <c r="F39" s="8" t="s">
         <v>70</v>
@@ -3863,13 +3866,13 @@
     </row>
     <row r="40" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" s="7">
-        <v>5940</v>
+        <v>5550</v>
       </c>
       <c r="C40" s="7">
-        <v>6390</v>
+        <v>5990</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="6"/>
@@ -3886,13 +3889,13 @@
     </row>
     <row r="41" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B41" s="7">
-        <v>5510</v>
+        <v>5940</v>
       </c>
       <c r="C41" s="7">
-        <v>5890</v>
+        <v>6390</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="6"/>
@@ -3902,9 +3905,15 @@
       <c r="I41" s="5"/>
     </row>
     <row r="42" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A42" s="8"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
+      <c r="A42" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="7">
+        <v>5510</v>
+      </c>
+      <c r="C42" s="7">
+        <v>5890</v>
+      </c>
       <c r="D42" s="5"/>
       <c r="E42" s="6"/>
       <c r="F42" s="8"/>

</xml_diff>

<commit_message>
12.10.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Price list September 2020.xlsx
+++ b/2020/Others/Price list September 2020.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="87">
   <si>
     <t>Model</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>D74</t>
+  </si>
+  <si>
+    <t>Md Masud Rana</t>
   </si>
 </sst>
 </file>
@@ -497,7 +500,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -535,15 +538,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -630,7 +624,7 @@
         <xdr:cNvPr id="2" name="Group 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -651,7 +645,7 @@
           <xdr:cNvPr id="3" name="Freeform 21">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -857,7 +851,7 @@
           <xdr:cNvPr id="4" name="Freeform 22">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1958,7 +1952,7 @@
           <xdr:cNvPr id="5" name="Freeform 23">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2405,7 +2399,7 @@
           <xdr:cNvPr id="6" name="Freeform 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2465,7 +2459,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2482,7 +2476,7 @@
           <xdr:cNvPr id="7" name="Freeform 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2545,7 +2539,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2562,7 +2556,7 @@
           <xdr:cNvPr id="8" name="Freeform 26">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2622,7 +2616,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2655,7 +2649,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2667,7 +2661,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2945,7 +2939,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2955,8 +2949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L46" sqref="L46"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2974,56 +2968,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
     </row>
     <row r="4" spans="1:15" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="34"/>
+      <c r="G4" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" s="30"/>
+      <c r="I4" s="31"/>
     </row>
     <row r="5" spans="1:15" ht="21" customHeight="1">
       <c r="A5" s="12" t="s">
@@ -3815,18 +3811,16 @@
       <c r="I37" s="5"/>
     </row>
     <row r="38" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="18">
+      <c r="B38" s="7">
         <v>5750</v>
       </c>
-      <c r="C38" s="18">
+      <c r="C38" s="7">
         <v>6190</v>
       </c>
-      <c r="D38" s="19">
-        <v>550</v>
-      </c>
+      <c r="D38" s="5"/>
       <c r="E38" s="6"/>
       <c r="F38" s="8" t="s">
         <v>80</v>
@@ -3944,33 +3938,33 @@
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="21" t="s">
+      <c r="A45" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="B45" s="22"/>
-      <c r="C45" s="22" t="s">
+      <c r="B45" s="19"/>
+      <c r="C45" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="D45" s="22"/>
-      <c r="E45" s="22"/>
-      <c r="F45" s="22"/>
-      <c r="G45" s="22"/>
-      <c r="H45" s="25" t="s">
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="I45" s="26"/>
+      <c r="I45" s="23"/>
       <c r="J45" s="2"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="23"/>
-      <c r="B46" s="24"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="24"/>
-      <c r="F46" s="24"/>
-      <c r="G46" s="24"/>
-      <c r="H46" s="27"/>
-      <c r="I46" s="28"/>
+      <c r="A46" s="20"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="24"/>
+      <c r="I46" s="25"/>
       <c r="J46" s="2"/>
     </row>
     <row r="47" spans="1:10">

</xml_diff>

<commit_message>
13.10.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Price list September 2020.xlsx
+++ b/2020/Others/Price list September 2020.xlsx
@@ -276,16 +276,16 @@
     <t xml:space="preserve">+8801312-116768 </t>
   </si>
   <si>
-    <t>DSR Name</t>
-  </si>
-  <si>
     <t xml:space="preserve">  </t>
   </si>
   <si>
     <t>D74</t>
   </si>
   <si>
-    <t>Md Masud Rana</t>
+    <t>HOT</t>
+  </si>
+  <si>
+    <t>October_2020</t>
   </si>
 </sst>
 </file>
@@ -371,7 +371,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -384,8 +384,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -494,13 +500,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -540,8 +559,14 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -579,10 +604,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2950,7 +2978,7 @@
   <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2968,58 +2996,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
     </row>
     <row r="4" spans="1:15" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="G4" s="30" t="s">
+      <c r="F4" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="H4" s="30"/>
-      <c r="I4" s="31"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="34"/>
     </row>
     <row r="5" spans="1:15" ht="21" customHeight="1">
       <c r="A5" s="12" t="s">
@@ -3259,7 +3285,7 @@
       </c>
       <c r="I14" s="5"/>
       <c r="K14" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="20.100000000000001" customHeight="1">
@@ -3574,7 +3600,7 @@
     </row>
     <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B28" s="7">
         <v>890</v>
@@ -3799,16 +3825,18 @@
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="6"/>
-      <c r="F37" s="8" t="s">
+      <c r="F37" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="G37" s="7">
-        <v>8310</v>
-      </c>
-      <c r="H37" s="7">
-        <v>8990</v>
-      </c>
-      <c r="I37" s="5"/>
+      <c r="G37" s="18">
+        <v>7800</v>
+      </c>
+      <c r="H37" s="18">
+        <v>8390</v>
+      </c>
+      <c r="I37" s="19" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="38" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="8" t="s">
@@ -3938,33 +3966,33 @@
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="18" t="s">
+      <c r="A45" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="B45" s="19"/>
-      <c r="C45" s="19" t="s">
+      <c r="B45" s="21"/>
+      <c r="C45" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="22" t="s">
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="I45" s="23"/>
+      <c r="I45" s="25"/>
       <c r="J45" s="2"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="20"/>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="24"/>
-      <c r="I46" s="25"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="27"/>
       <c r="J46" s="2"/>
     </row>
     <row r="47" spans="1:10">
@@ -3982,7 +4010,7 @@
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A4:D4"/>
-    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="F4:I4"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>